<commit_message>
[WIP] Fix WECC case
</commit_message>
<xml_diff>
--- a/ams/cases/wecc/wecc_uced.xlsx
+++ b/ams/cases/wecc/wecc_uced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/ams/ams/cases/wecc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98D8C98-265A-2F40-B29B-6C50BA0646E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD9973E-446C-CE46-971A-A5BD55C072E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21600" yWindow="2660" windowWidth="21600" windowHeight="18940" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21600" yWindow="2660" windowWidth="21600" windowHeight="18940" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="9" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2327" uniqueCount="1270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2329" uniqueCount="1271">
   <si>
     <t>idx</t>
   </si>
@@ -3860,6 +3860,9 @@
   </si>
   <si>
     <t>0.837, 0, 0</t>
+  </si>
+  <si>
+    <t>ctrl</t>
   </si>
 </sst>
 </file>
@@ -19839,16 +19842,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AG29"/>
+  <dimension ref="A1:AH29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L30" sqref="L30"/>
+      <selection pane="bottomLeft" activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -19901,55 +19904,58 @@
         <v>5</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>1270</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -20002,14 +20008,14 @@
         <v>0.6</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
         <v>0.3</v>
       </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
       <c r="U2">
         <v>0</v>
       </c>
@@ -20026,7 +20032,7 @@
         <v>0</v>
       </c>
       <c r="Z2">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="AA2">
         <v>999</v>
@@ -20035,7 +20041,7 @@
         <v>999</v>
       </c>
       <c r="AC2">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="AD2">
         <v>0</v>
@@ -20049,8 +20055,11 @@
       <c r="AG2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -20103,14 +20112,14 @@
         <v>0.6</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
         <v>0.3</v>
       </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
       <c r="U3">
         <v>0</v>
       </c>
@@ -20127,7 +20136,7 @@
         <v>0</v>
       </c>
       <c r="Z3">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="AA3">
         <v>999</v>
@@ -20136,7 +20145,7 @@
         <v>999</v>
       </c>
       <c r="AC3">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="AD3">
         <v>0</v>
@@ -20150,8 +20159,11 @@
       <c r="AG3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -20204,14 +20216,14 @@
         <v>0.6</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
         <v>0.3</v>
       </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
       <c r="U4">
         <v>0</v>
       </c>
@@ -20228,7 +20240,7 @@
         <v>0</v>
       </c>
       <c r="Z4">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="AA4">
         <v>999</v>
@@ -20237,7 +20249,7 @@
         <v>999</v>
       </c>
       <c r="AC4">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="AD4">
         <v>0</v>
@@ -20251,8 +20263,11 @@
       <c r="AG4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -20305,14 +20320,14 @@
         <v>0.6</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
         <v>0.3</v>
       </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
       <c r="U5">
         <v>0</v>
       </c>
@@ -20329,7 +20344,7 @@
         <v>0</v>
       </c>
       <c r="Z5">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="AA5">
         <v>999</v>
@@ -20338,7 +20353,7 @@
         <v>999</v>
       </c>
       <c r="AC5">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="AD5">
         <v>0</v>
@@ -20352,8 +20367,11 @@
       <c r="AG5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -20406,14 +20424,14 @@
         <v>0.6</v>
       </c>
       <c r="R6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
         <v>0.3</v>
       </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
       <c r="U6">
         <v>0</v>
       </c>
@@ -20430,7 +20448,7 @@
         <v>0</v>
       </c>
       <c r="Z6">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="AA6">
         <v>999</v>
@@ -20439,7 +20457,7 @@
         <v>999</v>
       </c>
       <c r="AC6">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="AD6">
         <v>0</v>
@@ -20453,8 +20471,11 @@
       <c r="AG6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -20507,14 +20528,14 @@
         <v>0.6</v>
       </c>
       <c r="R7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
         <v>0.3</v>
       </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
       <c r="U7">
         <v>0</v>
       </c>
@@ -20531,7 +20552,7 @@
         <v>0</v>
       </c>
       <c r="Z7">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="AA7">
         <v>999</v>
@@ -20540,7 +20561,7 @@
         <v>999</v>
       </c>
       <c r="AC7">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="AD7">
         <v>0</v>
@@ -20554,8 +20575,11 @@
       <c r="AG7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -20608,14 +20632,14 @@
         <v>0.6</v>
       </c>
       <c r="R8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
         <v>0.3</v>
       </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
       <c r="U8">
         <v>0</v>
       </c>
@@ -20632,7 +20656,7 @@
         <v>0</v>
       </c>
       <c r="Z8">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="AA8">
         <v>999</v>
@@ -20641,7 +20665,7 @@
         <v>999</v>
       </c>
       <c r="AC8">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="AD8">
         <v>0</v>
@@ -20655,8 +20679,11 @@
       <c r="AG8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -20709,14 +20736,14 @@
         <v>0.6</v>
       </c>
       <c r="R9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
         <v>0.3</v>
       </c>
-      <c r="T9">
-        <v>0</v>
-      </c>
       <c r="U9">
         <v>0</v>
       </c>
@@ -20733,7 +20760,7 @@
         <v>0</v>
       </c>
       <c r="Z9">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="AA9">
         <v>999</v>
@@ -20742,7 +20769,7 @@
         <v>999</v>
       </c>
       <c r="AC9">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="AD9">
         <v>0</v>
@@ -20756,8 +20783,11 @@
       <c r="AG9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -20810,14 +20840,14 @@
         <v>0.6</v>
       </c>
       <c r="R10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
         <v>0.3</v>
       </c>
-      <c r="T10">
-        <v>0</v>
-      </c>
       <c r="U10">
         <v>0</v>
       </c>
@@ -20834,7 +20864,7 @@
         <v>0</v>
       </c>
       <c r="Z10">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="AA10">
         <v>999</v>
@@ -20843,7 +20873,7 @@
         <v>999</v>
       </c>
       <c r="AC10">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="AD10">
         <v>0</v>
@@ -20857,8 +20887,11 @@
       <c r="AG10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -20911,14 +20944,14 @@
         <v>0.6</v>
       </c>
       <c r="R11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
         <v>0.3</v>
       </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
       <c r="U11">
         <v>0</v>
       </c>
@@ -20935,7 +20968,7 @@
         <v>0</v>
       </c>
       <c r="Z11">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="AA11">
         <v>999</v>
@@ -20944,7 +20977,7 @@
         <v>999</v>
       </c>
       <c r="AC11">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="AD11">
         <v>0</v>
@@ -20958,8 +20991,11 @@
       <c r="AG11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -21012,14 +21048,14 @@
         <v>0.6</v>
       </c>
       <c r="R12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
         <v>0.3</v>
       </c>
-      <c r="T12">
-        <v>0</v>
-      </c>
       <c r="U12">
         <v>0</v>
       </c>
@@ -21036,7 +21072,7 @@
         <v>0</v>
       </c>
       <c r="Z12">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="AA12">
         <v>999</v>
@@ -21045,7 +21081,7 @@
         <v>999</v>
       </c>
       <c r="AC12">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="AD12">
         <v>0</v>
@@ -21059,8 +21095,11 @@
       <c r="AG12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -21113,14 +21152,14 @@
         <v>0.6</v>
       </c>
       <c r="R13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
         <v>0.3</v>
       </c>
-      <c r="T13">
-        <v>0</v>
-      </c>
       <c r="U13">
         <v>0</v>
       </c>
@@ -21137,7 +21176,7 @@
         <v>0</v>
       </c>
       <c r="Z13">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="AA13">
         <v>999</v>
@@ -21146,7 +21185,7 @@
         <v>999</v>
       </c>
       <c r="AC13">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="AD13">
         <v>0</v>
@@ -21160,8 +21199,11 @@
       <c r="AG13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -21214,14 +21256,14 @@
         <v>0.6</v>
       </c>
       <c r="R14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
         <v>0.3</v>
       </c>
-      <c r="T14">
-        <v>0</v>
-      </c>
       <c r="U14">
         <v>0</v>
       </c>
@@ -21238,7 +21280,7 @@
         <v>0</v>
       </c>
       <c r="Z14">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="AA14">
         <v>999</v>
@@ -21247,7 +21289,7 @@
         <v>999</v>
       </c>
       <c r="AC14">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="AD14">
         <v>0</v>
@@ -21261,8 +21303,11 @@
       <c r="AG14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -21315,14 +21360,14 @@
         <v>0.6</v>
       </c>
       <c r="R15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
         <v>0.3</v>
       </c>
-      <c r="T15">
-        <v>0</v>
-      </c>
       <c r="U15">
         <v>0</v>
       </c>
@@ -21339,7 +21384,7 @@
         <v>0</v>
       </c>
       <c r="Z15">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="AA15">
         <v>999</v>
@@ -21348,7 +21393,7 @@
         <v>999</v>
       </c>
       <c r="AC15">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="AD15">
         <v>0</v>
@@ -21362,8 +21407,11 @@
       <c r="AG15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -21416,14 +21464,14 @@
         <v>0.6</v>
       </c>
       <c r="R16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
         <v>0.3</v>
       </c>
-      <c r="T16">
-        <v>0</v>
-      </c>
       <c r="U16">
         <v>0</v>
       </c>
@@ -21440,7 +21488,7 @@
         <v>0</v>
       </c>
       <c r="Z16">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="AA16">
         <v>999</v>
@@ -21449,7 +21497,7 @@
         <v>999</v>
       </c>
       <c r="AC16">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="AD16">
         <v>0</v>
@@ -21463,8 +21511,11 @@
       <c r="AG16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -21517,14 +21568,14 @@
         <v>0.6</v>
       </c>
       <c r="R17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
         <v>0.3</v>
       </c>
-      <c r="T17">
-        <v>0</v>
-      </c>
       <c r="U17">
         <v>0</v>
       </c>
@@ -21541,7 +21592,7 @@
         <v>0</v>
       </c>
       <c r="Z17">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="AA17">
         <v>999</v>
@@ -21550,7 +21601,7 @@
         <v>999</v>
       </c>
       <c r="AC17">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="AD17">
         <v>0</v>
@@ -21564,8 +21615,11 @@
       <c r="AG17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -21618,14 +21672,14 @@
         <v>0.6</v>
       </c>
       <c r="R18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
         <v>0.3</v>
       </c>
-      <c r="T18">
-        <v>0</v>
-      </c>
       <c r="U18">
         <v>0</v>
       </c>
@@ -21642,7 +21696,7 @@
         <v>0</v>
       </c>
       <c r="Z18">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="AA18">
         <v>999</v>
@@ -21651,7 +21705,7 @@
         <v>999</v>
       </c>
       <c r="AC18">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="AD18">
         <v>0</v>
@@ -21665,8 +21719,11 @@
       <c r="AG18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -21719,14 +21776,14 @@
         <v>0.6</v>
       </c>
       <c r="R19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
         <v>0.3</v>
       </c>
-      <c r="T19">
-        <v>0</v>
-      </c>
       <c r="U19">
         <v>0</v>
       </c>
@@ -21743,7 +21800,7 @@
         <v>0</v>
       </c>
       <c r="Z19">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="AA19">
         <v>999</v>
@@ -21752,7 +21809,7 @@
         <v>999</v>
       </c>
       <c r="AC19">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="AD19">
         <v>0</v>
@@ -21766,8 +21823,11 @@
       <c r="AG19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -21820,14 +21880,14 @@
         <v>0.6</v>
       </c>
       <c r="R20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
         <v>0.3</v>
       </c>
-      <c r="T20">
-        <v>0</v>
-      </c>
       <c r="U20">
         <v>0</v>
       </c>
@@ -21844,7 +21904,7 @@
         <v>0</v>
       </c>
       <c r="Z20">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="AA20">
         <v>999</v>
@@ -21853,7 +21913,7 @@
         <v>999</v>
       </c>
       <c r="AC20">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="AD20">
         <v>0</v>
@@ -21867,8 +21927,11 @@
       <c r="AG20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -21921,14 +21984,14 @@
         <v>0.6</v>
       </c>
       <c r="R21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
         <v>0.3</v>
       </c>
-      <c r="T21">
-        <v>0</v>
-      </c>
       <c r="U21">
         <v>0</v>
       </c>
@@ -21945,7 +22008,7 @@
         <v>0</v>
       </c>
       <c r="Z21">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="AA21">
         <v>999</v>
@@ -21954,7 +22017,7 @@
         <v>999</v>
       </c>
       <c r="AC21">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="AD21">
         <v>0</v>
@@ -21968,8 +22031,11 @@
       <c r="AG21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -22022,14 +22088,14 @@
         <v>0.6</v>
       </c>
       <c r="R22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22">
         <v>0.3</v>
       </c>
-      <c r="T22">
-        <v>0</v>
-      </c>
       <c r="U22">
         <v>0</v>
       </c>
@@ -22046,7 +22112,7 @@
         <v>0</v>
       </c>
       <c r="Z22">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="AA22">
         <v>999</v>
@@ -22055,7 +22121,7 @@
         <v>999</v>
       </c>
       <c r="AC22">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="AD22">
         <v>0</v>
@@ -22069,8 +22135,11 @@
       <c r="AG22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -22123,14 +22192,14 @@
         <v>0.6</v>
       </c>
       <c r="R23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
         <v>0.3</v>
       </c>
-      <c r="T23">
-        <v>0</v>
-      </c>
       <c r="U23">
         <v>0</v>
       </c>
@@ -22147,7 +22216,7 @@
         <v>0</v>
       </c>
       <c r="Z23">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="AA23">
         <v>999</v>
@@ -22156,7 +22225,7 @@
         <v>999</v>
       </c>
       <c r="AC23">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="AD23">
         <v>0</v>
@@ -22170,8 +22239,11 @@
       <c r="AG23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -22224,14 +22296,14 @@
         <v>0.6</v>
       </c>
       <c r="R24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
         <v>0.3</v>
       </c>
-      <c r="T24">
-        <v>0</v>
-      </c>
       <c r="U24">
         <v>0</v>
       </c>
@@ -22248,7 +22320,7 @@
         <v>0</v>
       </c>
       <c r="Z24">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="AA24">
         <v>999</v>
@@ -22257,7 +22329,7 @@
         <v>999</v>
       </c>
       <c r="AC24">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="AD24">
         <v>0</v>
@@ -22271,8 +22343,11 @@
       <c r="AG24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -22325,14 +22400,14 @@
         <v>0.6</v>
       </c>
       <c r="R25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="T25">
         <v>0.3</v>
       </c>
-      <c r="T25">
-        <v>0</v>
-      </c>
       <c r="U25">
         <v>0</v>
       </c>
@@ -22349,7 +22424,7 @@
         <v>0</v>
       </c>
       <c r="Z25">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="AA25">
         <v>999</v>
@@ -22358,7 +22433,7 @@
         <v>999</v>
       </c>
       <c r="AC25">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="AD25">
         <v>0</v>
@@ -22372,8 +22447,11 @@
       <c r="AG25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -22426,14 +22504,14 @@
         <v>0.6</v>
       </c>
       <c r="R26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="T26">
         <v>0.3</v>
       </c>
-      <c r="T26">
-        <v>0</v>
-      </c>
       <c r="U26">
         <v>0</v>
       </c>
@@ -22450,7 +22528,7 @@
         <v>0</v>
       </c>
       <c r="Z26">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="AA26">
         <v>999</v>
@@ -22459,7 +22537,7 @@
         <v>999</v>
       </c>
       <c r="AC26">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="AD26">
         <v>0</v>
@@ -22473,8 +22551,11 @@
       <c r="AG26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -22527,14 +22608,14 @@
         <v>0.6</v>
       </c>
       <c r="R27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
         <v>0.3</v>
       </c>
-      <c r="T27">
-        <v>0</v>
-      </c>
       <c r="U27">
         <v>0</v>
       </c>
@@ -22551,7 +22632,7 @@
         <v>0</v>
       </c>
       <c r="Z27">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="AA27">
         <v>999</v>
@@ -22560,7 +22641,7 @@
         <v>999</v>
       </c>
       <c r="AC27">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="AD27">
         <v>0</v>
@@ -22574,8 +22655,11 @@
       <c r="AG27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -22628,14 +22712,14 @@
         <v>0.6</v>
       </c>
       <c r="R28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28">
         <v>0.3</v>
       </c>
-      <c r="T28">
-        <v>0</v>
-      </c>
       <c r="U28">
         <v>0</v>
       </c>
@@ -22652,7 +22736,7 @@
         <v>0</v>
       </c>
       <c r="Z28">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="AA28">
         <v>999</v>
@@ -22661,7 +22745,7 @@
         <v>999</v>
       </c>
       <c r="AC28">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="AD28">
         <v>0</v>
@@ -22675,8 +22759,11 @@
       <c r="AG28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AH28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -22729,14 +22816,14 @@
         <v>0.6</v>
       </c>
       <c r="R29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S29">
+        <v>0</v>
+      </c>
+      <c r="T29">
         <v>0.3</v>
       </c>
-      <c r="T29">
-        <v>0</v>
-      </c>
       <c r="U29">
         <v>0</v>
       </c>
@@ -22753,7 +22840,7 @@
         <v>0</v>
       </c>
       <c r="Z29">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="AA29">
         <v>999</v>
@@ -22762,7 +22849,7 @@
         <v>999</v>
       </c>
       <c r="AC29">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="AD29">
         <v>0</v>
@@ -22774,6 +22861,9 @@
         <v>0</v>
       </c>
       <c r="AG29">
+        <v>0</v>
+      </c>
+      <c r="AH29">
         <v>0</v>
       </c>
     </row>
@@ -22785,16 +22875,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AH2"/>
+  <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
+      <selection pane="bottomLeft" activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -22847,58 +22937,61 @@
         <v>5</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>1270</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -22951,14 +23044,14 @@
         <v>0.6</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
         <v>0.3</v>
       </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
       <c r="U2">
         <v>0</v>
       </c>
@@ -22978,7 +23071,7 @@
         <v>0</v>
       </c>
       <c r="AA2">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="AB2">
         <v>999</v>
@@ -22987,7 +23080,7 @@
         <v>999</v>
       </c>
       <c r="AD2">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="AE2">
         <v>0</v>
@@ -22999,6 +23092,9 @@
         <v>0</v>
       </c>
       <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
         <v>0</v>
       </c>
     </row>

</xml_diff>